<commit_message>
update serial to parallel conversion and BPSK modulation
</commit_message>
<xml_diff>
--- a/doc/Work plan.xlsx
+++ b/doc/Work plan.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vista\Documents\semester 8\Digital Communication\Self-Learning-Projects\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vista\Documents\semester 8\Digital Communication\Self-Learning-Projects\basic_channel\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C39E605F-6227-4EC0-BFC0-86C5575DFDF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AA52943-B62E-4D3F-A6A9-10E1A2745D88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="37">
   <si>
     <t>ID</t>
   </si>
@@ -135,6 +135,12 @@
   </si>
   <si>
     <t>17/09/28</t>
+  </si>
+  <si>
+    <t>Bipolar nrz</t>
+  </si>
+  <si>
+    <t>Need S/P</t>
   </si>
 </sst>
 </file>
@@ -210,11 +216,11 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -520,7 +526,7 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -551,7 +557,7 @@
       <c r="E1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="9" t="s">
+      <c r="F1" s="8" t="s">
         <v>6</v>
       </c>
       <c r="G1" s="2" t="s">
@@ -571,7 +577,7 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="9" t="s">
         <v>10</v>
       </c>
       <c r="C2" t="s">
@@ -600,7 +606,7 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B3" s="8"/>
+      <c r="B3" s="9"/>
       <c r="C3" s="3" t="s">
         <v>12</v>
       </c>
@@ -627,7 +633,7 @@
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="9" t="s">
         <v>17</v>
       </c>
       <c r="C4" t="s">
@@ -639,18 +645,24 @@
       <c r="E4">
         <v>1</v>
       </c>
+      <c r="F4" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4">
+        <v>0.5</v>
+      </c>
       <c r="H4" t="s">
         <v>20</v>
       </c>
       <c r="I4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="J4" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="8"/>
+      <c r="B5" s="9"/>
       <c r="C5" t="s">
         <v>19</v>
       </c>
@@ -660,30 +672,51 @@
       <c r="E5">
         <v>1</v>
       </c>
+      <c r="F5" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="G5">
+        <v>0.5</v>
+      </c>
+      <c r="H5" s="7" t="s">
+        <v>35</v>
+      </c>
       <c r="I5" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="J5" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="8"/>
+      <c r="B6" s="9"/>
       <c r="C6" t="s">
         <v>22</v>
       </c>
       <c r="D6" s="7" t="s">
         <v>31</v>
       </c>
+      <c r="E6">
+        <v>2</v>
+      </c>
+      <c r="F6" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="G6">
+        <v>3</v>
+      </c>
+      <c r="H6" t="s">
+        <v>36</v>
+      </c>
       <c r="I6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="J6" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B7" s="8"/>
+      <c r="B7" s="9"/>
       <c r="C7" t="s">
         <v>23</v>
       </c>
@@ -698,7 +731,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="8"/>
+      <c r="B8" s="9"/>
       <c r="C8" t="s">
         <v>24</v>
       </c>

</xml_diff>

<commit_message>
Create a documentation on QPSK mod and demod, complete Matched filter demodulation
</commit_message>
<xml_diff>
--- a/doc/Work plan.xlsx
+++ b/doc/Work plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vista\Documents\semester 8\Digital Communication\Self-Learning-Projects\basic_channel\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AA52943-B62E-4D3F-A6A9-10E1A2745D88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C88E163-9977-4313-9BAB-6C472CF26401}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="37">
   <si>
     <t>ID</t>
   </si>
@@ -82,9 +82,6 @@
     <t>Todo</t>
   </si>
   <si>
-    <t>Create basic channel</t>
-  </si>
-  <si>
     <t>Generating bit stream</t>
   </si>
   <si>
@@ -92,12 +89,6 @@
   </si>
   <si>
     <t>Data rate : 1 bps</t>
-  </si>
-  <si>
-    <t>Binary ditector</t>
-  </si>
-  <si>
-    <t>BPSK modulator</t>
   </si>
   <si>
     <t>AWGN channel</t>
@@ -125,22 +116,32 @@
     <t>17/09/24</t>
   </si>
   <si>
-    <t>17/09/25</t>
-  </si>
-  <si>
-    <t>17/09/26</t>
-  </si>
-  <si>
-    <t>17/09/27</t>
-  </si>
-  <si>
-    <t>17/09/28</t>
-  </si>
-  <si>
     <t>Bipolar nrz</t>
   </si>
   <si>
     <t>Need S/P</t>
+  </si>
+  <si>
+    <t>QPSK modulator</t>
+  </si>
+  <si>
+    <t>QPSK PLL loop for carrier synchronization</t>
+  </si>
+  <si>
+    <t>23/09/21</t>
+  </si>
+  <si>
+    <t>24/09/21</t>
+  </si>
+  <si>
+    <t>Create basic  QPSK channel</t>
+  </si>
+  <si>
+    <t>Binary detector</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Matched filter detection
+Creating a documentation </t>
   </si>
 </sst>
 </file>
@@ -187,7 +188,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -195,22 +196,54 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -219,8 +252,44 @@
     <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -523,19 +592,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="31.42578125" customWidth="1"/>
     <col min="3" max="3" width="26.85546875" customWidth="1"/>
-    <col min="4" max="4" width="14.5703125" style="6" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" style="4" customWidth="1"/>
     <col min="5" max="5" width="14.42578125" customWidth="1"/>
-    <col min="6" max="6" width="12.7109375" style="7" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" style="5" customWidth="1"/>
     <col min="7" max="7" width="13.5703125" customWidth="1"/>
     <col min="8" max="8" width="37.42578125" customWidth="1"/>
     <col min="9" max="9" width="11.140625" customWidth="1"/>
@@ -551,13 +620,13 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="3" t="s">
         <v>4</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="F1" s="6" t="s">
         <v>6</v>
       </c>
       <c r="G1" s="2" t="s">
@@ -577,189 +646,229 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="B2" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="7">
+        <v>1</v>
+      </c>
+      <c r="F2" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="I2" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B3" s="17"/>
+      <c r="C3" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="12">
+        <v>1</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="H3" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="I3" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" s="12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B4" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="14">
+        <v>1</v>
+      </c>
+      <c r="F4" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" s="14">
+        <v>0.5</v>
+      </c>
+      <c r="H4" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="J4" s="14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B5" s="19"/>
+      <c r="C5" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E5" s="7">
+        <v>1</v>
+      </c>
+      <c r="F5" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="19"/>
+      <c r="C6" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="7">
+        <v>2</v>
+      </c>
+      <c r="F6" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="G2">
-        <v>0.5</v>
-      </c>
-      <c r="H2" t="s">
-        <v>25</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="G6" s="7">
+        <v>3</v>
+      </c>
+      <c r="H6" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="I6" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J6" s="7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B3" s="9"/>
-      <c r="C3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="G3">
-        <v>0.5</v>
-      </c>
-      <c r="H3" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="I3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J3" t="s">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B7" s="19"/>
+      <c r="C7" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="E7" s="7"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="7"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="J7" s="7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B4" s="9" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D4" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="G4">
-        <v>0.5</v>
-      </c>
-      <c r="H4" t="s">
-        <v>20</v>
-      </c>
-      <c r="I4" t="s">
-        <v>14</v>
-      </c>
-      <c r="J4" t="s">
+    <row r="8" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B8" s="19"/>
+      <c r="C8" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="D8" s="8"/>
+      <c r="E8" s="7"/>
+      <c r="F8" s="8"/>
+      <c r="G8" s="7"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="J8" s="7" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="9"/>
-      <c r="C5" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="G5">
-        <v>0.5</v>
-      </c>
-      <c r="H5" s="7" t="s">
+    <row r="9" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+      <c r="B9" s="19"/>
+      <c r="C9" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="21"/>
+      <c r="F9" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="G9" s="21"/>
+      <c r="H9" s="23" t="s">
+        <v>36</v>
+      </c>
+      <c r="I9" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="J9" s="21" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="20"/>
+      <c r="C10" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="I5" t="s">
-        <v>14</v>
-      </c>
-      <c r="J5" t="s">
+      <c r="D10" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="12"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12" t="s">
+        <v>13</v>
+      </c>
+      <c r="J10" s="12" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="9"/>
-      <c r="C6" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="E6">
-        <v>2</v>
-      </c>
-      <c r="F6" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="G6">
-        <v>3</v>
-      </c>
-      <c r="H6" t="s">
-        <v>36</v>
-      </c>
-      <c r="I6" t="s">
-        <v>14</v>
-      </c>
-      <c r="J6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B7" s="9"/>
-      <c r="C7" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="I7" t="s">
-        <v>16</v>
-      </c>
-      <c r="J7" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="9"/>
-      <c r="C8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>33</v>
-      </c>
-      <c r="I8" t="s">
-        <v>16</v>
-      </c>
-      <c r="J8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="C9" t="s">
-        <v>21</v>
-      </c>
-      <c r="D9" s="7" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B2:B3"/>
-    <mergeCell ref="B4:B8"/>
+    <mergeCell ref="B4:B10"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
-  <conditionalFormatting sqref="I2:I8">
+  <conditionalFormatting sqref="I2:I10">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
@@ -776,19 +885,19 @@
           <x14:formula1>
             <xm:f>Variables!$A$2:$A$3</xm:f>
           </x14:formula1>
-          <xm:sqref>I9:I12</xm:sqref>
+          <xm:sqref>I11:I13</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{D927ADCD-D976-446A-A5AF-DECABE737A23}">
           <x14:formula1>
             <xm:f>Variables!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>I2:I8</xm:sqref>
+          <xm:sqref>I2:I10</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{50E2DA23-DD80-49FE-B624-FDE87E63F771}">
           <x14:formula1>
             <xm:f>Variables!$B$2</xm:f>
           </x14:formula1>
-          <xm:sqref>J2:J8</xm:sqref>
+          <xm:sqref>J2:J10</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Add detection and BER calculation, update README.md
</commit_message>
<xml_diff>
--- a/doc/Work plan.xlsx
+++ b/doc/Work plan.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vista\Documents\semester 8\Digital Communication\Self-Learning-Projects\basic_channel\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C88E163-9977-4313-9BAB-6C472CF26401}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99E68D23-749B-41C6-8937-26668F699A69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="41">
   <si>
     <t>ID</t>
   </si>
@@ -142,6 +142,18 @@
   <si>
     <t xml:space="preserve">Matched filter detection
 Creating a documentation </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Need BER calculation </t>
+  </si>
+  <si>
+    <t>1 h</t>
+  </si>
+  <si>
+    <t>3 h</t>
+  </si>
+  <si>
+    <t>30 min</t>
   </si>
 </sst>
 </file>
@@ -238,7 +250,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -257,16 +269,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -282,14 +297,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -595,7 +613,7 @@
   <dimension ref="A1:J10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -646,7 +664,7 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="17" t="s">
         <v>10</v>
       </c>
       <c r="C2" s="7" t="s">
@@ -661,8 +679,8 @@
       <c r="F2" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="G2" s="7">
-        <v>0.5</v>
+      <c r="G2" s="7" t="s">
+        <v>40</v>
       </c>
       <c r="H2" s="7" t="s">
         <v>22</v>
@@ -674,64 +692,64 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B3" s="17"/>
-      <c r="C3" s="10" t="s">
+    <row r="3" spans="1:10" s="22" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B3" s="18"/>
+      <c r="C3" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="12">
+      <c r="E3" s="25">
         <v>1</v>
       </c>
-      <c r="F3" s="11" t="s">
+      <c r="F3" s="24" t="s">
         <v>24</v>
       </c>
-      <c r="G3" s="12">
-        <v>0.5</v>
-      </c>
-      <c r="H3" s="13" t="s">
+      <c r="G3" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="H3" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="I3" s="12" t="s">
+      <c r="I3" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="J3" s="12" t="s">
+      <c r="J3" s="25" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="D4" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="E4" s="14">
+      <c r="E4" s="12">
         <v>1</v>
       </c>
-      <c r="F4" s="15" t="s">
+      <c r="F4" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="G4" s="14">
-        <v>0.5</v>
-      </c>
-      <c r="H4" s="14" t="s">
+      <c r="G4" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="H4" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="I4" s="14" t="s">
+      <c r="I4" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="J4" s="14" t="s">
+      <c r="J4" s="12" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B5" s="19"/>
+      <c r="B5" s="20"/>
       <c r="C5" s="7" t="s">
         <v>18</v>
       </c>
@@ -744,8 +762,8 @@
       <c r="F5" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="G5" s="7">
-        <v>0.5</v>
+      <c r="G5" s="7" t="s">
+        <v>40</v>
       </c>
       <c r="H5" s="8" t="s">
         <v>28</v>
@@ -758,7 +776,7 @@
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B6" s="19"/>
+      <c r="B6" s="20"/>
       <c r="C6" s="7" t="s">
         <v>30</v>
       </c>
@@ -771,8 +789,8 @@
       <c r="F6" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="G6" s="7">
-        <v>3</v>
+      <c r="G6" s="7" t="s">
+        <v>39</v>
       </c>
       <c r="H6" s="7" t="s">
         <v>29</v>
@@ -785,7 +803,7 @@
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B7" s="19"/>
+      <c r="B7" s="20"/>
       <c r="C7" s="7" t="s">
         <v>20</v>
       </c>
@@ -804,7 +822,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B8" s="19"/>
+      <c r="B8" s="20"/>
       <c r="C8" s="9" t="s">
         <v>31</v>
       </c>
@@ -821,44 +839,52 @@
       </c>
     </row>
     <row r="9" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B9" s="19"/>
-      <c r="C9" s="21" t="s">
+      <c r="B9" s="20"/>
+      <c r="C9" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="22" t="s">
+      <c r="D9" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="E9" s="21"/>
-      <c r="F9" s="22" t="s">
+      <c r="E9" s="14"/>
+      <c r="F9" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="G9" s="21"/>
-      <c r="H9" s="23" t="s">
+      <c r="G9" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="H9" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="I9" s="21" t="s">
-        <v>13</v>
-      </c>
-      <c r="J9" s="21" t="s">
+      <c r="I9" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="J9" s="14" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B10" s="20"/>
-      <c r="C10" s="12" t="s">
+      <c r="B10" s="21"/>
+      <c r="C10" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="E10" s="12"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="12"/>
-      <c r="H10" s="12"/>
-      <c r="I10" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="J10" s="12" t="s">
+      <c r="E10" s="11"/>
+      <c r="F10" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="G10" s="11" t="s">
+        <v>40</v>
+      </c>
+      <c r="H10" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="I10" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="J10" s="11" t="s">
         <v>15</v>
       </c>
     </row>

</xml_diff>